<commit_message>
Modificado ej 4 y 8
</commit_message>
<xml_diff>
--- a/practica 2/diagramas/Ejer 4 diagramas.xlsx
+++ b/practica 2/diagramas/Ejer 4 diagramas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguspc\Desktop\facu\2do\2do semestre\ISO\practica 2\diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C625F2-53C9-464E-A4AC-49E1AED25A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE58B04-D2C9-4E3F-93AA-FB93FF348A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2353754-173D-4900-A564-D1A35AFCC5F7}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{F2353754-173D-4900-A564-D1A35AFCC5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:AY26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>